<commit_message>
iron mine test ok
</commit_message>
<xml_diff>
--- a/Client/assets/Csv/Building.xlsx
+++ b/Client/assets/Csv/Building.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\AnnoArk\Client\assets\Csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stvzhou/git/AnnoArk/Client/assets/Csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="85">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -178,10 +178,6 @@
   </si>
   <si>
     <t>iron83420</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>meal32872</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -360,8 +356,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -683,18 +679,18 @@
   <dimension ref="A1:AE19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="30" max="31" width="10.25" customWidth="1"/>
+    <col min="30" max="31" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -705,13 +701,13 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" t="s">
-        <v>44</v>
-      </c>
       <c r="F1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G1" t="s">
         <v>37</v>
@@ -783,13 +779,13 @@
         <v>19</v>
       </c>
       <c r="AD1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AE1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -804,7 +800,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -816,9 +812,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -831,7 +827,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -849,7 +845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -864,7 +860,7 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -876,7 +872,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -891,7 +887,7 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G5">
         <v>10</v>
@@ -903,12 +899,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -918,7 +914,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G6">
         <v>4</v>
@@ -945,12 +941,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -960,7 +956,7 @@
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -975,12 +971,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -989,7 +985,7 @@
         <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1007,7 +1003,7 @@
         <v>10</v>
       </c>
       <c r="L8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M8">
         <v>4</v>
@@ -1016,12 +1012,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -1031,7 +1027,7 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G9">
         <v>4</v>
@@ -1049,7 +1045,7 @@
         <v>5</v>
       </c>
       <c r="L9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M9">
         <v>2</v>
@@ -1061,12 +1057,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -1075,7 +1071,7 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G10">
         <v>6</v>
@@ -1099,12 +1095,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -1114,7 +1110,7 @@
         <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G11">
         <v>6</v>
@@ -1132,24 +1128,24 @@
         <v>5</v>
       </c>
       <c r="N11" t="s">
+        <v>74</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
+      </c>
+      <c r="V11" t="s">
         <v>75</v>
       </c>
-      <c r="O11">
-        <v>2</v>
-      </c>
-      <c r="V11" t="s">
-        <v>42</v>
-      </c>
       <c r="W11">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -1158,18 +1154,18 @@
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G12">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -1178,18 +1174,18 @@
         <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G13">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -1198,18 +1194,18 @@
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G14">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15">
         <v>4</v>
@@ -1218,18 +1214,18 @@
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G15">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -1238,18 +1234,18 @@
         <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G16">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D17">
         <v>5</v>
@@ -1258,18 +1254,18 @@
         <v>5</v>
       </c>
       <c r="F17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G17">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18">
         <v>4</v>
@@ -1278,52 +1274,52 @@
         <v>4</v>
       </c>
       <c r="F18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G18">
         <v>40</v>
       </c>
       <c r="N18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O18">
         <f>1000*W18</f>
         <v>16.666699999999999</v>
       </c>
       <c r="P18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q18">
         <f>10000*W18</f>
         <v>166.667</v>
       </c>
       <c r="R18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="S18">
         <f>200*W18</f>
         <v>3.3333399999999997</v>
       </c>
       <c r="T18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U18">
         <f>200*W18</f>
         <v>3.3333399999999997</v>
       </c>
       <c r="V18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="W18">
         <v>1.66667E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -1332,7 +1328,7 @@
         <v>3</v>
       </c>
       <c r="F19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G19">
         <v>20</v>

</xml_diff>

<commit_message>
a lot work, need to rethink
</commit_message>
<xml_diff>
--- a/Client/assets/Csv/Building.xlsx
+++ b/Client/assets/Csv/Building.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stvzhou/git/AnnoArk/Client/assets/Csv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\AnnoArk\Client\assets\Csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -181,14 +178,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>length</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>width</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>宿舍</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -350,6 +339,14 @@
   </si>
   <si>
     <t>fisher8032</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Width</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -357,7 +354,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -682,15 +679,15 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q11" sqref="Q11"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="30" max="31" width="10.1640625" customWidth="1"/>
+    <col min="30" max="31" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -701,13 +698,13 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="F1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G1" t="s">
         <v>37</v>
@@ -779,13 +776,13 @@
         <v>19</v>
       </c>
       <c r="AD1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AE1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -800,7 +797,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -812,9 +809,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -827,7 +824,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -845,7 +842,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -860,7 +857,7 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -872,7 +869,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -887,7 +884,7 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G5">
         <v>10</v>
@@ -899,12 +896,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31">
       <c r="A6" t="s">
         <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -914,7 +911,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G6">
         <v>4</v>
@@ -941,12 +938,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -956,7 +953,7 @@
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -971,12 +968,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -985,7 +982,7 @@
         <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1003,7 +1000,7 @@
         <v>10</v>
       </c>
       <c r="L8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M8">
         <v>4</v>
@@ -1012,12 +1009,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31">
       <c r="A9" t="s">
         <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -1027,7 +1024,7 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G9">
         <v>4</v>
@@ -1045,7 +1042,7 @@
         <v>5</v>
       </c>
       <c r="L9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M9">
         <v>2</v>
@@ -1057,12 +1054,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -1071,7 +1068,7 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G10">
         <v>6</v>
@@ -1095,12 +1092,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -1110,7 +1107,7 @@
         <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G11">
         <v>6</v>
@@ -1128,24 +1125,24 @@
         <v>5</v>
       </c>
       <c r="N11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="O11">
         <v>2</v>
       </c>
       <c r="V11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="W11">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -1154,18 +1151,18 @@
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G12">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -1174,18 +1171,18 @@
         <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G13">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -1194,18 +1191,18 @@
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G14">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D15">
         <v>4</v>
@@ -1214,18 +1211,18 @@
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G15">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -1234,18 +1231,18 @@
         <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G16">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D17">
         <v>5</v>
@@ -1254,18 +1251,18 @@
         <v>5</v>
       </c>
       <c r="F17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G17">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D18">
         <v>4</v>
@@ -1274,52 +1271,52 @@
         <v>4</v>
       </c>
       <c r="F18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G18">
         <v>40</v>
       </c>
       <c r="N18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O18">
         <f>1000*W18</f>
         <v>16.666699999999999</v>
       </c>
       <c r="P18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Q18">
         <f>10000*W18</f>
         <v>166.667</v>
       </c>
       <c r="R18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S18">
         <f>200*W18</f>
         <v>3.3333399999999997</v>
       </c>
       <c r="T18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="U18">
         <f>200*W18</f>
         <v>3.3333399999999997</v>
       </c>
       <c r="V18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="W18">
         <v>1.66667E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -1328,7 +1325,7 @@
         <v>3</v>
       </c>
       <c r="F19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G19">
         <v>20</v>

</xml_diff>